<commit_message>
Implement general update to PIXdb codes
</commit_message>
<xml_diff>
--- a/pixdb_backoffice/data/outliers_summary.xlsx
+++ b/pixdb_backoffice/data/outliers_summary.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26812"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marzec01/data/PhD/Transcriptomics_project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Library/WebServer/Documents/PIXdb/pixdb_backoffice/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6478BB05-A5E2-6E4B-AD97-6C207690D116}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27620" yWindow="460" windowWidth="21620" windowHeight="20540" tabRatio="500"/>
+    <workbookView xWindow="3940" yWindow="480" windowWidth="21620" windowHeight="16200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datasets" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Datasets!$B$1:$N$74</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -865,8 +866,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="13">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2456,7 +2457,52 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2465,53 +2511,299 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="40" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="50" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="42" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="49" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2519,27 +2811,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2548,276 +2819,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="49" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="50" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="42" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="40" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="601">
@@ -3562,6 +3563,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -3887,8 +3891,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:N77"/>
@@ -3900,7 +3904,7 @@
       <selection pane="bottomRight" activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="5.6640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="16.6640625" style="2" customWidth="1"/>
@@ -3918,7 +3922,7 @@
     <col min="15" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="4" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" s="4" customFormat="1" ht="40" customHeight="1">
       <c r="A1" s="17"/>
       <c r="B1" s="18" t="s">
         <v>92</v>
@@ -3960,26 +3964,26 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="159" t="s">
+    <row r="2" spans="1:14" ht="27" customHeight="1">
+      <c r="A2" s="131" t="s">
         <v>90</v>
       </c>
-      <c r="B2" s="98" t="s">
+      <c r="B2" s="73" t="s">
         <v>93</v>
       </c>
-      <c r="C2" s="162" t="s">
+      <c r="C2" s="135" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="100">
+      <c r="D2" s="159">
         <v>550</v>
       </c>
-      <c r="E2" s="100" t="s">
+      <c r="E2" s="159" t="s">
         <v>3</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="G2" s="100" t="s">
+      <c r="G2" s="159" t="s">
         <v>0</v>
       </c>
       <c r="H2" s="37">
@@ -3995,26 +3999,26 @@
         <f t="shared" ref="K2:K13" si="0">SUM(H2:J2)</f>
         <v>0</v>
       </c>
-      <c r="L2" s="100" t="s">
+      <c r="L2" s="159" t="s">
         <v>62</v>
       </c>
-      <c r="M2" s="109" t="s">
-        <v>0</v>
-      </c>
-      <c r="N2" s="98" t="s">
+      <c r="M2" s="175" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" s="73" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="159"/>
-      <c r="B3" s="99"/>
-      <c r="C3" s="163"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
+    <row r="3" spans="1:14" ht="27" customHeight="1">
+      <c r="A3" s="131"/>
+      <c r="B3" s="170"/>
+      <c r="C3" s="136"/>
+      <c r="D3" s="160"/>
+      <c r="E3" s="160"/>
       <c r="F3" s="22" t="s">
         <v>156</v>
       </c>
-      <c r="G3" s="76"/>
+      <c r="G3" s="160"/>
       <c r="H3" s="41">
         <v>1</v>
       </c>
@@ -4028,20 +4032,20 @@
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="L3" s="76"/>
-      <c r="M3" s="110"/>
-      <c r="N3" s="179"/>
-    </row>
-    <row r="4" spans="1:14" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="159"/>
-      <c r="B4" s="65"/>
-      <c r="C4" s="164"/>
-      <c r="D4" s="101"/>
-      <c r="E4" s="101"/>
+      <c r="L3" s="160"/>
+      <c r="M3" s="151"/>
+      <c r="N3" s="74"/>
+    </row>
+    <row r="4" spans="1:14" ht="26" customHeight="1">
+      <c r="A4" s="131"/>
+      <c r="B4" s="80"/>
+      <c r="C4" s="137"/>
+      <c r="D4" s="161"/>
+      <c r="E4" s="161"/>
       <c r="F4" s="22" t="s">
         <v>157</v>
       </c>
-      <c r="G4" s="101"/>
+      <c r="G4" s="161"/>
       <c r="H4" s="38">
         <v>0</v>
       </c>
@@ -4055,26 +4059,26 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="L4" s="101"/>
-      <c r="M4" s="111"/>
-      <c r="N4" s="180"/>
-    </row>
-    <row r="5" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="159"/>
-      <c r="B5" s="65"/>
-      <c r="C5" s="105" t="s">
+      <c r="L4" s="161"/>
+      <c r="M4" s="176"/>
+      <c r="N4" s="75"/>
+    </row>
+    <row r="5" spans="1:14" ht="27" customHeight="1">
+      <c r="A5" s="131"/>
+      <c r="B5" s="80"/>
+      <c r="C5" s="174" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="82">
+      <c r="D5" s="146">
         <v>12</v>
       </c>
-      <c r="E5" s="82" t="s">
+      <c r="E5" s="146" t="s">
         <v>3</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="G5" s="82" t="s">
+      <c r="G5" s="146" t="s">
         <v>0</v>
       </c>
       <c r="H5" s="33">
@@ -4090,26 +4094,26 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="L5" s="82" t="s">
+      <c r="L5" s="146" t="s">
         <v>63</v>
       </c>
-      <c r="M5" s="107" t="s">
+      <c r="M5" s="153" t="s">
         <v>19</v>
       </c>
-      <c r="N5" s="102" t="s">
+      <c r="N5" s="171" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="159"/>
-      <c r="B6" s="66"/>
-      <c r="C6" s="106"/>
-      <c r="D6" s="79"/>
-      <c r="E6" s="79"/>
+    <row r="6" spans="1:14" ht="27" customHeight="1">
+      <c r="A6" s="131"/>
+      <c r="B6" s="81"/>
+      <c r="C6" s="109"/>
+      <c r="D6" s="85"/>
+      <c r="E6" s="85"/>
       <c r="F6" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="G6" s="79"/>
+      <c r="G6" s="85"/>
       <c r="H6" s="30">
         <v>0</v>
       </c>
@@ -4123,28 +4127,28 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L6" s="79"/>
-      <c r="M6" s="108"/>
-      <c r="N6" s="112"/>
-    </row>
-    <row r="7" spans="1:14" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="159"/>
-      <c r="B7" s="64" t="s">
+      <c r="L6" s="85"/>
+      <c r="M6" s="93"/>
+      <c r="N6" s="177"/>
+    </row>
+    <row r="7" spans="1:14" ht="34" customHeight="1">
+      <c r="A7" s="131"/>
+      <c r="B7" s="79" t="s">
         <v>99</v>
       </c>
-      <c r="C7" s="161" t="s">
+      <c r="C7" s="133" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="115">
+      <c r="D7" s="100">
         <v>30</v>
       </c>
-      <c r="E7" s="115" t="s">
+      <c r="E7" s="100" t="s">
         <v>3</v>
       </c>
       <c r="F7" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="G7" s="115" t="s">
+      <c r="G7" s="100" t="s">
         <v>0</v>
       </c>
       <c r="H7" s="56">
@@ -4160,26 +4164,26 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="L7" s="115" t="s">
+      <c r="L7" s="100" t="s">
         <v>63</v>
       </c>
-      <c r="M7" s="184" t="s">
-        <v>0</v>
-      </c>
-      <c r="N7" s="131" t="s">
+      <c r="M7" s="103" t="s">
+        <v>0</v>
+      </c>
+      <c r="N7" s="167" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="160"/>
-      <c r="B8" s="66"/>
-      <c r="C8" s="90"/>
-      <c r="D8" s="96"/>
-      <c r="E8" s="96"/>
+    <row r="8" spans="1:14" ht="34" customHeight="1">
+      <c r="A8" s="132"/>
+      <c r="B8" s="81"/>
+      <c r="C8" s="134"/>
+      <c r="D8" s="87"/>
+      <c r="E8" s="87"/>
       <c r="F8" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="G8" s="96"/>
+      <c r="G8" s="87"/>
       <c r="H8" s="57">
         <v>10</v>
       </c>
@@ -4193,30 +4197,30 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="L8" s="96"/>
-      <c r="M8" s="135"/>
-      <c r="N8" s="132"/>
-    </row>
-    <row r="9" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="165" t="s">
+      <c r="L8" s="87"/>
+      <c r="M8" s="104"/>
+      <c r="N8" s="168"/>
+    </row>
+    <row r="9" spans="1:14" ht="27" customHeight="1">
+      <c r="A9" s="138" t="s">
         <v>91</v>
       </c>
-      <c r="B9" s="64" t="s">
+      <c r="B9" s="79" t="s">
         <v>100</v>
       </c>
-      <c r="C9" s="70" t="s">
+      <c r="C9" s="157" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="80">
+      <c r="D9" s="101">
         <v>179</v>
       </c>
-      <c r="E9" s="80" t="s">
+      <c r="E9" s="101" t="s">
         <v>3</v>
       </c>
       <c r="F9" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="G9" s="152" t="s">
+      <c r="G9" s="94" t="s">
         <v>73</v>
       </c>
       <c r="H9" s="31">
@@ -4232,26 +4236,26 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="L9" s="80" t="s">
+      <c r="L9" s="101" t="s">
         <v>64</v>
       </c>
-      <c r="M9" s="143" t="s">
-        <v>0</v>
-      </c>
-      <c r="N9" s="113" t="s">
+      <c r="M9" s="91" t="s">
+        <v>0</v>
+      </c>
+      <c r="N9" s="78" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="166"/>
-      <c r="B10" s="65"/>
-      <c r="C10" s="71"/>
-      <c r="D10" s="78"/>
-      <c r="E10" s="78"/>
+    <row r="10" spans="1:14" ht="27" customHeight="1">
+      <c r="A10" s="139"/>
+      <c r="B10" s="80"/>
+      <c r="C10" s="178"/>
+      <c r="D10" s="84"/>
+      <c r="E10" s="84"/>
       <c r="F10" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="G10" s="145"/>
+      <c r="G10" s="92"/>
       <c r="H10" s="29">
         <v>7</v>
       </c>
@@ -4265,20 +4269,20 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="L10" s="78"/>
-      <c r="M10" s="145"/>
-      <c r="N10" s="120"/>
-    </row>
-    <row r="11" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="166"/>
-      <c r="B11" s="65"/>
-      <c r="C11" s="72"/>
-      <c r="D11" s="116"/>
-      <c r="E11" s="116"/>
+      <c r="L10" s="84"/>
+      <c r="M10" s="92"/>
+      <c r="N10" s="68"/>
+    </row>
+    <row r="11" spans="1:14" ht="27" customHeight="1">
+      <c r="A11" s="139"/>
+      <c r="B11" s="80"/>
+      <c r="C11" s="179"/>
+      <c r="D11" s="102"/>
+      <c r="E11" s="102"/>
       <c r="F11" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="G11" s="181"/>
+      <c r="G11" s="95"/>
       <c r="H11" s="45">
         <v>0</v>
       </c>
@@ -4292,26 +4296,26 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="L11" s="116"/>
-      <c r="M11" s="181"/>
-      <c r="N11" s="133"/>
-    </row>
-    <row r="12" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="166"/>
-      <c r="B12" s="88"/>
-      <c r="C12" s="93" t="s">
+      <c r="L11" s="102"/>
+      <c r="M11" s="95"/>
+      <c r="N11" s="169"/>
+    </row>
+    <row r="12" spans="1:14" ht="27" customHeight="1">
+      <c r="A12" s="139"/>
+      <c r="B12" s="117"/>
+      <c r="C12" s="183" t="s">
         <v>47</v>
       </c>
-      <c r="D12" s="117">
+      <c r="D12" s="107">
         <v>95</v>
       </c>
-      <c r="E12" s="117" t="s">
+      <c r="E12" s="107" t="s">
         <v>3</v>
       </c>
       <c r="F12" s="46" t="s">
         <v>140</v>
       </c>
-      <c r="G12" s="182" t="s">
+      <c r="G12" s="96" t="s">
         <v>0</v>
       </c>
       <c r="H12" s="47">
@@ -4327,26 +4331,26 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="L12" s="117" t="s">
+      <c r="L12" s="107" t="s">
         <v>64</v>
       </c>
-      <c r="M12" s="122" t="s">
-        <v>0</v>
-      </c>
-      <c r="N12" s="146" t="s">
+      <c r="M12" s="163" t="s">
+        <v>0</v>
+      </c>
+      <c r="N12" s="154" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="166"/>
-      <c r="B13" s="88"/>
-      <c r="C13" s="94"/>
-      <c r="D13" s="118"/>
-      <c r="E13" s="118"/>
+    <row r="13" spans="1:14" ht="27" customHeight="1">
+      <c r="A13" s="139"/>
+      <c r="B13" s="117"/>
+      <c r="C13" s="184"/>
+      <c r="D13" s="97"/>
+      <c r="E13" s="97"/>
       <c r="F13" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="G13" s="118"/>
+      <c r="G13" s="97"/>
       <c r="H13" s="49">
         <v>4</v>
       </c>
@@ -4360,26 +4364,26 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="L13" s="118"/>
-      <c r="M13" s="123"/>
-      <c r="N13" s="147"/>
-    </row>
-    <row r="14" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="166"/>
-      <c r="B14" s="65"/>
-      <c r="C14" s="170" t="s">
+      <c r="L13" s="97"/>
+      <c r="M13" s="164"/>
+      <c r="N13" s="155"/>
+    </row>
+    <row r="14" spans="1:14" ht="27" customHeight="1">
+      <c r="A14" s="139"/>
+      <c r="B14" s="80"/>
+      <c r="C14" s="108" t="s">
         <v>70</v>
       </c>
-      <c r="D14" s="97">
+      <c r="D14" s="110">
         <v>48</v>
       </c>
-      <c r="E14" s="97" t="s">
+      <c r="E14" s="110" t="s">
         <v>3</v>
       </c>
       <c r="F14" s="39" t="s">
         <v>135</v>
       </c>
-      <c r="G14" s="183" t="s">
+      <c r="G14" s="98" t="s">
         <v>74</v>
       </c>
       <c r="H14" s="40">
@@ -4395,26 +4399,26 @@
         <f>SUM(H14:J14)</f>
         <v>0</v>
       </c>
-      <c r="L14" s="97" t="s">
+      <c r="L14" s="110" t="s">
         <v>64</v>
       </c>
-      <c r="M14" s="149" t="s">
-        <v>0</v>
-      </c>
-      <c r="N14" s="150" t="s">
+      <c r="M14" s="113" t="s">
+        <v>0</v>
+      </c>
+      <c r="N14" s="114" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="166"/>
-      <c r="B15" s="65"/>
-      <c r="C15" s="156"/>
-      <c r="D15" s="81"/>
-      <c r="E15" s="81"/>
+    <row r="15" spans="1:14" ht="27" customHeight="1">
+      <c r="A15" s="139"/>
+      <c r="B15" s="80"/>
+      <c r="C15" s="148"/>
+      <c r="D15" s="119"/>
+      <c r="E15" s="119"/>
       <c r="F15" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="G15" s="144"/>
+      <c r="G15" s="99"/>
       <c r="H15" s="32">
         <v>2</v>
       </c>
@@ -4428,26 +4432,26 @@
         <f t="shared" ref="K15:K22" si="1">SUM(H15:J15)</f>
         <v>4</v>
       </c>
-      <c r="L15" s="81"/>
-      <c r="M15" s="144"/>
-      <c r="N15" s="114"/>
-    </row>
-    <row r="16" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="166"/>
-      <c r="B16" s="65"/>
-      <c r="C16" s="89" t="s">
+      <c r="L15" s="119"/>
+      <c r="M15" s="99"/>
+      <c r="N15" s="69"/>
+    </row>
+    <row r="16" spans="1:14" ht="27" customHeight="1">
+      <c r="A16" s="139"/>
+      <c r="B16" s="80"/>
+      <c r="C16" s="158" t="s">
         <v>130</v>
       </c>
-      <c r="D16" s="95">
+      <c r="D16" s="149">
         <v>22</v>
       </c>
-      <c r="E16" s="91" t="s">
+      <c r="E16" s="86" t="s">
         <v>3</v>
       </c>
       <c r="F16" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="G16" s="91" t="s">
+      <c r="G16" s="86" t="s">
         <v>0</v>
       </c>
       <c r="H16" s="36">
@@ -4463,26 +4467,26 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="L16" s="95" t="s">
+      <c r="L16" s="149" t="s">
         <v>64</v>
       </c>
-      <c r="M16" s="134" t="s">
-        <v>0</v>
-      </c>
-      <c r="N16" s="124" t="s">
+      <c r="M16" s="152" t="s">
+        <v>0</v>
+      </c>
+      <c r="N16" s="165" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="166"/>
-      <c r="B17" s="66"/>
-      <c r="C17" s="90"/>
-      <c r="D17" s="96"/>
-      <c r="E17" s="92"/>
+    <row r="17" spans="1:14" ht="27" customHeight="1">
+      <c r="A17" s="139"/>
+      <c r="B17" s="81"/>
+      <c r="C17" s="134"/>
+      <c r="D17" s="87"/>
+      <c r="E17" s="182"/>
       <c r="F17" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="G17" s="96"/>
+      <c r="G17" s="87"/>
       <c r="H17" s="35">
         <v>1</v>
       </c>
@@ -4496,28 +4500,28 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="L17" s="96"/>
-      <c r="M17" s="135"/>
-      <c r="N17" s="125"/>
-    </row>
-    <row r="18" spans="1:14" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="166"/>
-      <c r="B18" s="64" t="s">
+      <c r="L17" s="87"/>
+      <c r="M17" s="104"/>
+      <c r="N17" s="166"/>
+    </row>
+    <row r="18" spans="1:14" s="6" customFormat="1" ht="27" customHeight="1">
+      <c r="A18" s="139"/>
+      <c r="B18" s="79" t="s">
         <v>94</v>
       </c>
-      <c r="C18" s="70" t="s">
+      <c r="C18" s="157" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="80">
+      <c r="D18" s="101">
         <v>80</v>
       </c>
-      <c r="E18" s="80" t="s">
+      <c r="E18" s="101" t="s">
         <v>3</v>
       </c>
       <c r="F18" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="G18" s="80" t="s">
+      <c r="G18" s="101" t="s">
         <v>0</v>
       </c>
       <c r="H18" s="52">
@@ -4533,26 +4537,26 @@
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="L18" s="80" t="s">
-        <v>0</v>
-      </c>
-      <c r="M18" s="143" t="s">
-        <v>0</v>
-      </c>
-      <c r="N18" s="113" t="s">
+      <c r="L18" s="101" t="s">
+        <v>0</v>
+      </c>
+      <c r="M18" s="91" t="s">
+        <v>0</v>
+      </c>
+      <c r="N18" s="78" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="19" spans="1:14" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="166"/>
-      <c r="B19" s="65"/>
-      <c r="C19" s="156"/>
-      <c r="D19" s="81"/>
-      <c r="E19" s="81"/>
+    <row r="19" spans="1:14" s="6" customFormat="1" ht="27" customHeight="1">
+      <c r="A19" s="139"/>
+      <c r="B19" s="80"/>
+      <c r="C19" s="148"/>
+      <c r="D19" s="119"/>
+      <c r="E19" s="119"/>
       <c r="F19" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="G19" s="81"/>
+      <c r="G19" s="119"/>
       <c r="H19" s="55">
         <v>40</v>
       </c>
@@ -4566,26 +4570,26 @@
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="L19" s="81"/>
-      <c r="M19" s="144"/>
-      <c r="N19" s="114"/>
-    </row>
-    <row r="20" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="166"/>
-      <c r="B20" s="65"/>
-      <c r="C20" s="89" t="s">
+      <c r="L19" s="119"/>
+      <c r="M19" s="99"/>
+      <c r="N19" s="69"/>
+    </row>
+    <row r="20" spans="1:14" ht="27" customHeight="1">
+      <c r="A20" s="139"/>
+      <c r="B20" s="80"/>
+      <c r="C20" s="158" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="95">
+      <c r="D20" s="149">
         <v>116</v>
       </c>
-      <c r="E20" s="91" t="s">
+      <c r="E20" s="86" t="s">
         <v>3</v>
       </c>
       <c r="F20" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="G20" s="95" t="s">
+      <c r="G20" s="149" t="s">
         <v>0</v>
       </c>
       <c r="H20" s="36">
@@ -4601,26 +4605,26 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="L20" s="95" t="s">
+      <c r="L20" s="149" t="s">
         <v>68</v>
       </c>
-      <c r="M20" s="134" t="s">
-        <v>0</v>
-      </c>
-      <c r="N20" s="148" t="s">
+      <c r="M20" s="152" t="s">
+        <v>0</v>
+      </c>
+      <c r="N20" s="156" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="166"/>
-      <c r="B21" s="65"/>
-      <c r="C21" s="89"/>
-      <c r="D21" s="95"/>
-      <c r="E21" s="91"/>
+    <row r="21" spans="1:14" ht="27" customHeight="1">
+      <c r="A21" s="139"/>
+      <c r="B21" s="80"/>
+      <c r="C21" s="158"/>
+      <c r="D21" s="149"/>
+      <c r="E21" s="86"/>
       <c r="F21" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="G21" s="95"/>
+      <c r="G21" s="149"/>
       <c r="H21" s="36">
         <v>2</v>
       </c>
@@ -4634,20 +4638,20 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="L21" s="95"/>
-      <c r="M21" s="134"/>
-      <c r="N21" s="148"/>
-    </row>
-    <row r="22" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="166"/>
-      <c r="B22" s="65"/>
-      <c r="C22" s="89"/>
-      <c r="D22" s="95"/>
-      <c r="E22" s="91"/>
+      <c r="L21" s="149"/>
+      <c r="M21" s="152"/>
+      <c r="N21" s="156"/>
+    </row>
+    <row r="22" spans="1:14" ht="27" customHeight="1">
+      <c r="A22" s="139"/>
+      <c r="B22" s="80"/>
+      <c r="C22" s="158"/>
+      <c r="D22" s="149"/>
+      <c r="E22" s="86"/>
       <c r="F22" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="G22" s="95"/>
+      <c r="G22" s="149"/>
       <c r="H22" s="36">
         <v>4</v>
       </c>
@@ -4661,26 +4665,26 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="L22" s="95"/>
-      <c r="M22" s="134"/>
-      <c r="N22" s="148"/>
-    </row>
-    <row r="23" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="166"/>
-      <c r="B23" s="65"/>
-      <c r="C23" s="140" t="s">
+      <c r="L22" s="149"/>
+      <c r="M22" s="152"/>
+      <c r="N22" s="156"/>
+    </row>
+    <row r="23" spans="1:14" ht="27" customHeight="1">
+      <c r="A23" s="139"/>
+      <c r="B23" s="80"/>
+      <c r="C23" s="70" t="s">
         <v>42</v>
       </c>
-      <c r="D23" s="82">
+      <c r="D23" s="146">
         <v>81</v>
       </c>
-      <c r="E23" s="82" t="s">
+      <c r="E23" s="146" t="s">
         <v>3</v>
       </c>
       <c r="F23" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="G23" s="82" t="s">
+      <c r="G23" s="146" t="s">
         <v>0</v>
       </c>
       <c r="H23" s="33">
@@ -4696,26 +4700,26 @@
         <f t="shared" ref="K23:K28" si="2">SUM(H23:J23)</f>
         <v>6</v>
       </c>
-      <c r="L23" s="85" t="s">
+      <c r="L23" s="162" t="s">
         <v>65</v>
       </c>
-      <c r="M23" s="107" t="s">
-        <v>0</v>
-      </c>
-      <c r="N23" s="102" t="s">
+      <c r="M23" s="153" t="s">
+        <v>0</v>
+      </c>
+      <c r="N23" s="171" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="166"/>
-      <c r="B24" s="65"/>
-      <c r="C24" s="141"/>
-      <c r="D24" s="78"/>
-      <c r="E24" s="78"/>
+    <row r="24" spans="1:14" ht="27" customHeight="1">
+      <c r="A24" s="139"/>
+      <c r="B24" s="80"/>
+      <c r="C24" s="71"/>
+      <c r="D24" s="84"/>
+      <c r="E24" s="84"/>
       <c r="F24" s="16" t="s">
         <v>167</v>
       </c>
-      <c r="G24" s="78"/>
+      <c r="G24" s="84"/>
       <c r="H24" s="29">
         <v>3</v>
       </c>
@@ -4729,20 +4733,20 @@
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="L24" s="78"/>
-      <c r="M24" s="145"/>
-      <c r="N24" s="103"/>
-    </row>
-    <row r="25" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="166"/>
-      <c r="B25" s="65"/>
-      <c r="C25" s="142"/>
-      <c r="D25" s="81"/>
-      <c r="E25" s="81"/>
+      <c r="L24" s="84"/>
+      <c r="M24" s="92"/>
+      <c r="N24" s="172"/>
+    </row>
+    <row r="25" spans="1:14" ht="27" customHeight="1">
+      <c r="A25" s="139"/>
+      <c r="B25" s="80"/>
+      <c r="C25" s="72"/>
+      <c r="D25" s="119"/>
+      <c r="E25" s="119"/>
       <c r="F25" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="G25" s="81"/>
+      <c r="G25" s="119"/>
       <c r="H25" s="51">
         <v>2</v>
       </c>
@@ -4756,26 +4760,26 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="L25" s="81"/>
-      <c r="M25" s="144"/>
-      <c r="N25" s="104"/>
-    </row>
-    <row r="26" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="166"/>
-      <c r="B26" s="65"/>
-      <c r="C26" s="67" t="s">
+      <c r="L25" s="119"/>
+      <c r="M25" s="99"/>
+      <c r="N25" s="173"/>
+    </row>
+    <row r="26" spans="1:14" ht="27" customHeight="1">
+      <c r="A26" s="139"/>
+      <c r="B26" s="80"/>
+      <c r="C26" s="105" t="s">
         <v>71</v>
       </c>
-      <c r="D26" s="68">
+      <c r="D26" s="147">
         <v>19</v>
       </c>
-      <c r="E26" s="69" t="s">
+      <c r="E26" s="129" t="s">
         <v>9</v>
       </c>
       <c r="F26" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="G26" s="69" t="s">
+      <c r="G26" s="129" t="s">
         <v>0</v>
       </c>
       <c r="H26" s="28">
@@ -4791,26 +4795,26 @@
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="L26" s="69" t="s">
+      <c r="L26" s="129" t="s">
         <v>65</v>
       </c>
-      <c r="M26" s="151" t="s">
-        <v>0</v>
-      </c>
-      <c r="N26" s="126" t="s">
+      <c r="M26" s="82" t="s">
+        <v>0</v>
+      </c>
+      <c r="N26" s="66" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="166"/>
-      <c r="B27" s="65"/>
-      <c r="C27" s="67"/>
-      <c r="D27" s="68"/>
-      <c r="E27" s="69"/>
+    <row r="27" spans="1:14" ht="27" customHeight="1">
+      <c r="A27" s="139"/>
+      <c r="B27" s="80"/>
+      <c r="C27" s="105"/>
+      <c r="D27" s="147"/>
+      <c r="E27" s="129"/>
       <c r="F27" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="G27" s="69"/>
+      <c r="G27" s="129"/>
       <c r="H27" s="28">
         <v>1</v>
       </c>
@@ -4824,26 +4828,26 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="L27" s="68"/>
-      <c r="M27" s="151"/>
-      <c r="N27" s="126"/>
-    </row>
-    <row r="28" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="166"/>
-      <c r="B28" s="65"/>
-      <c r="C28" s="140" t="s">
+      <c r="L27" s="147"/>
+      <c r="M27" s="82"/>
+      <c r="N27" s="66"/>
+    </row>
+    <row r="28" spans="1:14" ht="27" customHeight="1">
+      <c r="A28" s="139"/>
+      <c r="B28" s="80"/>
+      <c r="C28" s="70" t="s">
         <v>131</v>
       </c>
-      <c r="D28" s="82">
+      <c r="D28" s="146">
         <v>19</v>
       </c>
-      <c r="E28" s="85" t="s">
+      <c r="E28" s="162" t="s">
         <v>9</v>
       </c>
       <c r="F28" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="G28" s="128" t="s">
+      <c r="G28" s="88" t="s">
         <v>75</v>
       </c>
       <c r="H28" s="33">
@@ -4859,26 +4863,26 @@
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="L28" s="85" t="s">
+      <c r="L28" s="162" t="s">
         <v>65</v>
       </c>
-      <c r="M28" s="128" t="s">
+      <c r="M28" s="88" t="s">
         <v>84</v>
       </c>
-      <c r="N28" s="178" t="s">
+      <c r="N28" s="67" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="166"/>
-      <c r="B29" s="65"/>
-      <c r="C29" s="141"/>
-      <c r="D29" s="78"/>
-      <c r="E29" s="86"/>
+    <row r="29" spans="1:14" ht="27" customHeight="1">
+      <c r="A29" s="139"/>
+      <c r="B29" s="80"/>
+      <c r="C29" s="71"/>
+      <c r="D29" s="84"/>
+      <c r="E29" s="121"/>
       <c r="F29" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="G29" s="129"/>
+      <c r="G29" s="89"/>
       <c r="H29" s="29">
         <v>2</v>
       </c>
@@ -4892,20 +4896,20 @@
         <f t="shared" ref="K29:K48" si="3">SUM(H29:J29)</f>
         <v>2</v>
       </c>
-      <c r="L29" s="78"/>
-      <c r="M29" s="129"/>
-      <c r="N29" s="120"/>
-    </row>
-    <row r="30" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="166"/>
-      <c r="B30" s="65"/>
-      <c r="C30" s="142"/>
-      <c r="D30" s="81"/>
-      <c r="E30" s="87"/>
+      <c r="L29" s="84"/>
+      <c r="M29" s="89"/>
+      <c r="N29" s="68"/>
+    </row>
+    <row r="30" spans="1:14" ht="27" customHeight="1">
+      <c r="A30" s="139"/>
+      <c r="B30" s="80"/>
+      <c r="C30" s="72"/>
+      <c r="D30" s="119"/>
+      <c r="E30" s="120"/>
       <c r="F30" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="G30" s="130"/>
+      <c r="G30" s="90"/>
       <c r="H30" s="32">
         <v>0</v>
       </c>
@@ -4919,26 +4923,26 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="L30" s="81"/>
-      <c r="M30" s="130"/>
-      <c r="N30" s="114"/>
-    </row>
-    <row r="31" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="166"/>
-      <c r="B31" s="65"/>
-      <c r="C31" s="67" t="s">
+      <c r="L30" s="119"/>
+      <c r="M30" s="90"/>
+      <c r="N30" s="69"/>
+    </row>
+    <row r="31" spans="1:14" ht="27" customHeight="1">
+      <c r="A31" s="139"/>
+      <c r="B31" s="80"/>
+      <c r="C31" s="105" t="s">
         <v>39</v>
       </c>
-      <c r="D31" s="68">
+      <c r="D31" s="147">
         <v>11</v>
       </c>
-      <c r="E31" s="68" t="s">
+      <c r="E31" s="147" t="s">
         <v>3</v>
       </c>
       <c r="F31" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="G31" s="151" t="s">
+      <c r="G31" s="82" t="s">
         <v>76</v>
       </c>
       <c r="H31" s="28">
@@ -4954,26 +4958,26 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="L31" s="69" t="s">
+      <c r="L31" s="129" t="s">
         <v>65</v>
       </c>
-      <c r="M31" s="151" t="s">
-        <v>0</v>
-      </c>
-      <c r="N31" s="126" t="s">
+      <c r="M31" s="82" t="s">
+        <v>0</v>
+      </c>
+      <c r="N31" s="66" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="166"/>
-      <c r="B32" s="65"/>
-      <c r="C32" s="67"/>
-      <c r="D32" s="68"/>
-      <c r="E32" s="68"/>
+    <row r="32" spans="1:14" ht="27" customHeight="1">
+      <c r="A32" s="139"/>
+      <c r="B32" s="80"/>
+      <c r="C32" s="105"/>
+      <c r="D32" s="147"/>
+      <c r="E32" s="147"/>
       <c r="F32" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="G32" s="151"/>
+      <c r="G32" s="82"/>
       <c r="H32" s="28">
         <v>0</v>
       </c>
@@ -4987,20 +4991,20 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L32" s="68"/>
-      <c r="M32" s="151"/>
-      <c r="N32" s="126"/>
-    </row>
-    <row r="33" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="166"/>
-      <c r="B33" s="66"/>
-      <c r="C33" s="158"/>
-      <c r="D33" s="74"/>
-      <c r="E33" s="74"/>
+      <c r="L32" s="147"/>
+      <c r="M32" s="82"/>
+      <c r="N32" s="66"/>
+    </row>
+    <row r="33" spans="1:14" ht="27" customHeight="1">
+      <c r="A33" s="139"/>
+      <c r="B33" s="81"/>
+      <c r="C33" s="106"/>
+      <c r="D33" s="130"/>
+      <c r="E33" s="130"/>
       <c r="F33" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="G33" s="138"/>
+      <c r="G33" s="77"/>
       <c r="H33" s="27">
         <v>0</v>
       </c>
@@ -5014,28 +5018,28 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L33" s="74"/>
-      <c r="M33" s="138"/>
-      <c r="N33" s="127"/>
-    </row>
-    <row r="34" spans="1:14" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="166"/>
-      <c r="B34" s="64" t="s">
+      <c r="L33" s="130"/>
+      <c r="M33" s="77"/>
+      <c r="N33" s="65"/>
+    </row>
+    <row r="34" spans="1:14" ht="29" customHeight="1">
+      <c r="A34" s="139"/>
+      <c r="B34" s="79" t="s">
         <v>95</v>
       </c>
-      <c r="C34" s="153" t="s">
+      <c r="C34" s="118" t="s">
         <v>50</v>
       </c>
-      <c r="D34" s="80">
+      <c r="D34" s="101">
         <v>89</v>
       </c>
-      <c r="E34" s="77" t="s">
+      <c r="E34" s="83" t="s">
         <v>3</v>
       </c>
       <c r="F34" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="G34" s="77" t="s">
+      <c r="G34" s="83" t="s">
         <v>0</v>
       </c>
       <c r="H34" s="31">
@@ -5051,26 +5055,26 @@
         <f t="shared" si="3"/>
         <v>69</v>
       </c>
-      <c r="L34" s="77" t="s">
+      <c r="L34" s="83" t="s">
         <v>69</v>
       </c>
-      <c r="M34" s="143" t="s">
-        <v>0</v>
-      </c>
-      <c r="N34" s="113" t="s">
+      <c r="M34" s="91" t="s">
+        <v>0</v>
+      </c>
+      <c r="N34" s="78" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="166"/>
-      <c r="B35" s="65"/>
-      <c r="C35" s="141"/>
-      <c r="D35" s="78"/>
-      <c r="E35" s="86"/>
+    <row r="35" spans="1:14" ht="29" customHeight="1">
+      <c r="A35" s="139"/>
+      <c r="B35" s="80"/>
+      <c r="C35" s="71"/>
+      <c r="D35" s="84"/>
+      <c r="E35" s="121"/>
       <c r="F35" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="G35" s="78"/>
+      <c r="G35" s="84"/>
       <c r="H35" s="29">
         <v>10</v>
       </c>
@@ -5084,20 +5088,20 @@
         <f t="shared" si="3"/>
         <v>18</v>
       </c>
-      <c r="L35" s="78"/>
-      <c r="M35" s="145"/>
-      <c r="N35" s="120"/>
-    </row>
-    <row r="36" spans="1:14" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="166"/>
-      <c r="B36" s="66"/>
-      <c r="C36" s="154"/>
-      <c r="D36" s="79"/>
-      <c r="E36" s="155"/>
+      <c r="L35" s="84"/>
+      <c r="M35" s="92"/>
+      <c r="N35" s="68"/>
+    </row>
+    <row r="36" spans="1:14" ht="29" customHeight="1">
+      <c r="A36" s="139"/>
+      <c r="B36" s="81"/>
+      <c r="C36" s="143"/>
+      <c r="D36" s="85"/>
+      <c r="E36" s="112"/>
       <c r="F36" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="G36" s="79"/>
+      <c r="G36" s="85"/>
       <c r="H36" s="30">
         <v>0</v>
       </c>
@@ -5111,29 +5115,29 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="L36" s="79"/>
-      <c r="M36" s="108"/>
-      <c r="N36" s="121"/>
-    </row>
-    <row r="37" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="166"/>
-      <c r="B37" s="64" t="s">
+      <c r="L36" s="85"/>
+      <c r="M36" s="93"/>
+      <c r="N36" s="115"/>
+    </row>
+    <row r="37" spans="1:14" ht="33" customHeight="1">
+      <c r="A37" s="139"/>
+      <c r="B37" s="79" t="s">
         <v>168</v>
       </c>
-      <c r="C37" s="157" t="s">
+      <c r="C37" s="142" t="s">
         <v>53</v>
       </c>
-      <c r="D37" s="83">
+      <c r="D37" s="180">
         <f>57 * 2</f>
         <v>114</v>
       </c>
-      <c r="E37" s="73" t="s">
+      <c r="E37" s="144" t="s">
         <v>3</v>
       </c>
       <c r="F37" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="G37" s="73" t="s">
+      <c r="G37" s="144" t="s">
         <v>0</v>
       </c>
       <c r="H37" s="34">
@@ -5149,26 +5153,26 @@
         <f t="shared" si="3"/>
         <v>72</v>
       </c>
-      <c r="L37" s="73" t="s">
+      <c r="L37" s="144" t="s">
         <v>65</v>
       </c>
-      <c r="M37" s="137" t="s">
-        <v>0</v>
-      </c>
-      <c r="N37" s="177" t="s">
+      <c r="M37" s="76" t="s">
+        <v>0</v>
+      </c>
+      <c r="N37" s="64" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="166"/>
-      <c r="B38" s="66"/>
-      <c r="C38" s="158"/>
-      <c r="D38" s="84"/>
-      <c r="E38" s="119"/>
+    <row r="38" spans="1:14" ht="33" customHeight="1">
+      <c r="A38" s="139"/>
+      <c r="B38" s="81"/>
+      <c r="C38" s="106"/>
+      <c r="D38" s="181"/>
+      <c r="E38" s="145"/>
       <c r="F38" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="G38" s="119"/>
+      <c r="G38" s="145"/>
       <c r="H38" s="27">
         <v>8</v>
       </c>
@@ -5182,28 +5186,28 @@
         <f t="shared" si="3"/>
         <v>17</v>
       </c>
-      <c r="L38" s="74"/>
-      <c r="M38" s="138"/>
-      <c r="N38" s="127"/>
-    </row>
-    <row r="39" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="166"/>
-      <c r="B39" s="64" t="s">
+      <c r="L38" s="130"/>
+      <c r="M38" s="77"/>
+      <c r="N38" s="65"/>
+    </row>
+    <row r="39" spans="1:14" ht="30" customHeight="1">
+      <c r="A39" s="139"/>
+      <c r="B39" s="79" t="s">
         <v>96</v>
       </c>
-      <c r="C39" s="153" t="s">
+      <c r="C39" s="118" t="s">
         <v>72</v>
       </c>
-      <c r="D39" s="80">
+      <c r="D39" s="101">
         <v>106</v>
       </c>
-      <c r="E39" s="77" t="s">
+      <c r="E39" s="83" t="s">
         <v>9</v>
       </c>
       <c r="F39" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="G39" s="77" t="s">
+      <c r="G39" s="83" t="s">
         <v>0</v>
       </c>
       <c r="H39" s="31">
@@ -5219,26 +5223,26 @@
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="L39" s="80" t="s">
+      <c r="L39" s="101" t="s">
         <v>68</v>
       </c>
-      <c r="M39" s="152" t="s">
-        <v>0</v>
-      </c>
-      <c r="N39" s="113" t="s">
+      <c r="M39" s="94" t="s">
+        <v>0</v>
+      </c>
+      <c r="N39" s="78" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="166"/>
-      <c r="B40" s="65"/>
-      <c r="C40" s="142"/>
-      <c r="D40" s="81"/>
-      <c r="E40" s="87"/>
+    <row r="40" spans="1:14" ht="30" customHeight="1">
+      <c r="A40" s="139"/>
+      <c r="B40" s="80"/>
+      <c r="C40" s="72"/>
+      <c r="D40" s="119"/>
+      <c r="E40" s="120"/>
       <c r="F40" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="G40" s="81"/>
+      <c r="G40" s="119"/>
       <c r="H40" s="32">
         <v>11</v>
       </c>
@@ -5252,26 +5256,26 @@
         <f t="shared" si="3"/>
         <v>19</v>
       </c>
-      <c r="L40" s="81"/>
-      <c r="M40" s="130"/>
-      <c r="N40" s="114"/>
-    </row>
-    <row r="41" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="166"/>
-      <c r="B41" s="65"/>
-      <c r="C41" s="67" t="s">
+      <c r="L40" s="119"/>
+      <c r="M40" s="90"/>
+      <c r="N40" s="69"/>
+    </row>
+    <row r="41" spans="1:14" ht="30" customHeight="1">
+      <c r="A41" s="139"/>
+      <c r="B41" s="80"/>
+      <c r="C41" s="105" t="s">
         <v>54</v>
       </c>
-      <c r="D41" s="68">
+      <c r="D41" s="147">
         <v>51</v>
       </c>
-      <c r="E41" s="69" t="s">
+      <c r="E41" s="129" t="s">
         <v>3</v>
       </c>
       <c r="F41" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="G41" s="65" t="s">
+      <c r="G41" s="80" t="s">
         <v>77</v>
       </c>
       <c r="H41" s="28">
@@ -5287,26 +5291,26 @@
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="L41" s="69" t="s">
+      <c r="L41" s="129" t="s">
         <v>65</v>
       </c>
-      <c r="M41" s="65" t="s">
+      <c r="M41" s="80" t="s">
         <v>85</v>
       </c>
-      <c r="N41" s="126" t="s">
+      <c r="N41" s="66" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="166"/>
-      <c r="B42" s="66"/>
-      <c r="C42" s="158"/>
-      <c r="D42" s="74"/>
-      <c r="E42" s="119"/>
+    <row r="42" spans="1:14" ht="30" customHeight="1">
+      <c r="A42" s="139"/>
+      <c r="B42" s="81"/>
+      <c r="C42" s="106"/>
+      <c r="D42" s="130"/>
+      <c r="E42" s="145"/>
       <c r="F42" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="G42" s="66"/>
+      <c r="G42" s="81"/>
       <c r="H42" s="27">
         <v>5</v>
       </c>
@@ -5320,29 +5324,29 @@
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="L42" s="74"/>
-      <c r="M42" s="66"/>
-      <c r="N42" s="127"/>
-    </row>
-    <row r="43" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="166"/>
-      <c r="B43" s="64" t="s">
+      <c r="L42" s="130"/>
+      <c r="M42" s="81"/>
+      <c r="N42" s="65"/>
+    </row>
+    <row r="43" spans="1:14" ht="33" customHeight="1">
+      <c r="A43" s="139"/>
+      <c r="B43" s="79" t="s">
         <v>101</v>
       </c>
-      <c r="C43" s="153" t="s">
+      <c r="C43" s="118" t="s">
         <v>55</v>
       </c>
-      <c r="D43" s="80">
+      <c r="D43" s="101">
         <f>163 * 3</f>
         <v>489</v>
       </c>
-      <c r="E43" s="77" t="s">
+      <c r="E43" s="83" t="s">
         <v>3</v>
       </c>
       <c r="F43" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="G43" s="152" t="s">
+      <c r="G43" s="94" t="s">
         <v>78</v>
       </c>
       <c r="H43" s="31">
@@ -5358,26 +5362,26 @@
         <f t="shared" si="3"/>
         <v>30</v>
       </c>
-      <c r="L43" s="77" t="s">
+      <c r="L43" s="83" t="s">
         <v>65</v>
       </c>
-      <c r="M43" s="152" t="s">
+      <c r="M43" s="94" t="s">
         <v>84</v>
       </c>
-      <c r="N43" s="113" t="s">
+      <c r="N43" s="78" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="166"/>
-      <c r="B44" s="65"/>
-      <c r="C44" s="141"/>
-      <c r="D44" s="78"/>
-      <c r="E44" s="86"/>
+    <row r="44" spans="1:14" ht="33" customHeight="1">
+      <c r="A44" s="139"/>
+      <c r="B44" s="80"/>
+      <c r="C44" s="71"/>
+      <c r="D44" s="84"/>
+      <c r="E44" s="121"/>
       <c r="F44" s="16" t="s">
         <v>161</v>
       </c>
-      <c r="G44" s="129"/>
+      <c r="G44" s="89"/>
       <c r="H44" s="29">
         <v>60</v>
       </c>
@@ -5391,20 +5395,20 @@
         <f t="shared" si="3"/>
         <v>138</v>
       </c>
-      <c r="L44" s="78"/>
-      <c r="M44" s="129"/>
-      <c r="N44" s="120"/>
-    </row>
-    <row r="45" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="166"/>
-      <c r="B45" s="65"/>
-      <c r="C45" s="141"/>
-      <c r="D45" s="78"/>
-      <c r="E45" s="86"/>
+      <c r="L44" s="84"/>
+      <c r="M44" s="89"/>
+      <c r="N44" s="68"/>
+    </row>
+    <row r="45" spans="1:14" ht="33" customHeight="1">
+      <c r="A45" s="139"/>
+      <c r="B45" s="80"/>
+      <c r="C45" s="71"/>
+      <c r="D45" s="84"/>
+      <c r="E45" s="121"/>
       <c r="F45" s="16" t="s">
         <v>162</v>
       </c>
-      <c r="G45" s="129"/>
+      <c r="G45" s="89"/>
       <c r="H45" s="29">
         <v>45</v>
       </c>
@@ -5418,20 +5422,20 @@
         <f t="shared" si="3"/>
         <v>90</v>
       </c>
-      <c r="L45" s="78"/>
-      <c r="M45" s="129"/>
-      <c r="N45" s="120"/>
-    </row>
-    <row r="46" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="166"/>
-      <c r="B46" s="66"/>
-      <c r="C46" s="154"/>
-      <c r="D46" s="79"/>
-      <c r="E46" s="155"/>
+      <c r="L45" s="84"/>
+      <c r="M45" s="89"/>
+      <c r="N45" s="68"/>
+    </row>
+    <row r="46" spans="1:14" ht="33" customHeight="1">
+      <c r="A46" s="139"/>
+      <c r="B46" s="81"/>
+      <c r="C46" s="143"/>
+      <c r="D46" s="85"/>
+      <c r="E46" s="112"/>
       <c r="F46" s="15" t="s">
         <v>163</v>
       </c>
-      <c r="G46" s="172"/>
+      <c r="G46" s="122"/>
       <c r="H46" s="30">
         <v>18</v>
       </c>
@@ -5445,28 +5449,28 @@
         <f t="shared" si="3"/>
         <v>30</v>
       </c>
-      <c r="L46" s="79"/>
-      <c r="M46" s="172"/>
-      <c r="N46" s="121"/>
-    </row>
-    <row r="47" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="166"/>
-      <c r="B47" s="171" t="s">
+      <c r="L46" s="85"/>
+      <c r="M46" s="122"/>
+      <c r="N46" s="115"/>
+    </row>
+    <row r="47" spans="1:14" ht="27" customHeight="1">
+      <c r="A47" s="139"/>
+      <c r="B47" s="116" t="s">
         <v>97</v>
       </c>
-      <c r="C47" s="173" t="s">
+      <c r="C47" s="123" t="s">
         <v>79</v>
       </c>
-      <c r="D47" s="83">
+      <c r="D47" s="180">
         <v>102</v>
       </c>
-      <c r="E47" s="75" t="s">
+      <c r="E47" s="125" t="s">
         <v>9</v>
       </c>
       <c r="F47" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="G47" s="75" t="s">
+      <c r="G47" s="125" t="s">
         <v>0</v>
       </c>
       <c r="H47" s="34">
@@ -5482,26 +5486,26 @@
         <f t="shared" si="3"/>
         <v>34</v>
       </c>
-      <c r="L47" s="75" t="s">
+      <c r="L47" s="125" t="s">
         <v>65</v>
       </c>
-      <c r="M47" s="139" t="s">
-        <v>0</v>
-      </c>
-      <c r="N47" s="175" t="s">
+      <c r="M47" s="150" t="s">
+        <v>0</v>
+      </c>
+      <c r="N47" s="127" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="166"/>
-      <c r="B48" s="88"/>
-      <c r="C48" s="174"/>
-      <c r="D48" s="76"/>
-      <c r="E48" s="168"/>
+    <row r="48" spans="1:14" ht="27" customHeight="1">
+      <c r="A48" s="139"/>
+      <c r="B48" s="117"/>
+      <c r="C48" s="124"/>
+      <c r="D48" s="160"/>
+      <c r="E48" s="126"/>
       <c r="F48" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="G48" s="168"/>
+      <c r="G48" s="126"/>
       <c r="H48" s="38">
         <v>6</v>
       </c>
@@ -5515,26 +5519,26 @@
         <f t="shared" si="3"/>
         <v>27</v>
       </c>
-      <c r="L48" s="76"/>
-      <c r="M48" s="110"/>
-      <c r="N48" s="176"/>
-    </row>
-    <row r="49" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="166"/>
-      <c r="B49" s="65"/>
-      <c r="C49" s="170" t="s">
+      <c r="L48" s="160"/>
+      <c r="M48" s="151"/>
+      <c r="N48" s="128"/>
+    </row>
+    <row r="49" spans="1:14" ht="27" customHeight="1">
+      <c r="A49" s="139"/>
+      <c r="B49" s="80"/>
+      <c r="C49" s="108" t="s">
         <v>81</v>
       </c>
-      <c r="D49" s="97">
+      <c r="D49" s="110">
         <v>88</v>
       </c>
-      <c r="E49" s="169" t="s">
+      <c r="E49" s="111" t="s">
         <v>9</v>
       </c>
       <c r="F49" s="39" t="s">
         <v>153</v>
       </c>
-      <c r="G49" s="169" t="s">
+      <c r="G49" s="111" t="s">
         <v>0</v>
       </c>
       <c r="H49" s="40">
@@ -5550,26 +5554,26 @@
         <f>SUM(H49:J49)</f>
         <v>26</v>
       </c>
-      <c r="L49" s="97" t="s">
+      <c r="L49" s="110" t="s">
         <v>65</v>
       </c>
-      <c r="M49" s="149" t="s">
-        <v>0</v>
-      </c>
-      <c r="N49" s="150" t="s">
+      <c r="M49" s="113" t="s">
+        <v>0</v>
+      </c>
+      <c r="N49" s="114" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="166"/>
-      <c r="B50" s="66"/>
-      <c r="C50" s="106"/>
-      <c r="D50" s="79"/>
-      <c r="E50" s="155"/>
+    <row r="50" spans="1:14" ht="27" customHeight="1">
+      <c r="A50" s="139"/>
+      <c r="B50" s="81"/>
+      <c r="C50" s="109"/>
+      <c r="D50" s="85"/>
+      <c r="E50" s="112"/>
       <c r="F50" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="G50" s="155"/>
+      <c r="G50" s="112"/>
       <c r="H50" s="30">
         <v>5</v>
       </c>
@@ -5583,28 +5587,28 @@
         <f>SUM(H50:J50)</f>
         <v>5</v>
       </c>
-      <c r="L50" s="79"/>
-      <c r="M50" s="108"/>
-      <c r="N50" s="121"/>
-    </row>
-    <row r="51" spans="1:14" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="166"/>
-      <c r="B51" s="64" t="s">
+      <c r="L50" s="85"/>
+      <c r="M50" s="93"/>
+      <c r="N50" s="115"/>
+    </row>
+    <row r="51" spans="1:14" ht="32" customHeight="1">
+      <c r="A51" s="139"/>
+      <c r="B51" s="79" t="s">
         <v>98</v>
       </c>
-      <c r="C51" s="157" t="s">
+      <c r="C51" s="142" t="s">
         <v>5</v>
       </c>
-      <c r="D51" s="136">
+      <c r="D51" s="141">
         <v>98</v>
       </c>
-      <c r="E51" s="136" t="s">
+      <c r="E51" s="141" t="s">
         <v>3</v>
       </c>
       <c r="F51" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="G51" s="136" t="s">
+      <c r="G51" s="141" t="s">
         <v>0</v>
       </c>
       <c r="H51" s="34">
@@ -5620,26 +5624,26 @@
         <f>SUM(H51:J51)</f>
         <v>6</v>
       </c>
-      <c r="L51" s="73" t="s">
+      <c r="L51" s="144" t="s">
         <v>66</v>
       </c>
-      <c r="M51" s="137" t="s">
-        <v>0</v>
-      </c>
-      <c r="N51" s="64" t="s">
+      <c r="M51" s="76" t="s">
+        <v>0</v>
+      </c>
+      <c r="N51" s="79" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="167"/>
-      <c r="B52" s="66"/>
-      <c r="C52" s="158"/>
-      <c r="D52" s="74"/>
-      <c r="E52" s="74"/>
+    <row r="52" spans="1:14" ht="35" customHeight="1">
+      <c r="A52" s="140"/>
+      <c r="B52" s="81"/>
+      <c r="C52" s="106"/>
+      <c r="D52" s="130"/>
+      <c r="E52" s="130"/>
       <c r="F52" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="G52" s="74"/>
+      <c r="G52" s="130"/>
       <c r="H52" s="27">
         <v>1</v>
       </c>
@@ -5653,17 +5657,17 @@
         <f>SUM(H52:J52)</f>
         <v>3</v>
       </c>
-      <c r="L52" s="119"/>
-      <c r="M52" s="138"/>
-      <c r="N52" s="66"/>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L52" s="145"/>
+      <c r="M52" s="77"/>
+      <c r="N52" s="81"/>
+    </row>
+    <row r="53" spans="1:14">
       <c r="A53" s="1"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
       <c r="N53" s="1"/>
     </row>
-    <row r="54" spans="1:14" s="61" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" s="61" customFormat="1" ht="19">
       <c r="B54" s="62"/>
       <c r="C54" s="61" t="s">
         <v>172</v>
@@ -5693,7 +5697,7 @@
       </c>
       <c r="M54" s="62"/>
     </row>
-    <row r="55" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" ht="19">
       <c r="A55" s="1" t="s">
         <v>88</v>
       </c>
@@ -5720,7 +5724,7 @@
       <c r="K55" s="61"/>
       <c r="N55" s="1"/>
     </row>
-    <row r="56" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" ht="19">
       <c r="A56" s="1" t="s">
         <v>86</v>
       </c>
@@ -5739,7 +5743,7 @@
       <c r="K56" s="61"/>
       <c r="N56" s="1"/>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14">
       <c r="A57" s="1" t="s">
         <v>79</v>
       </c>
@@ -5750,7 +5754,7 @@
       <c r="E57" s="1"/>
       <c r="N57" s="1"/>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14">
       <c r="A58" s="1" t="s">
         <v>18</v>
       </c>
@@ -5761,7 +5765,7 @@
       <c r="E58" s="1"/>
       <c r="N58" s="1"/>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14">
       <c r="A59" s="1" t="s">
         <v>103</v>
       </c>
@@ -5772,7 +5776,7 @@
       <c r="E59" s="1"/>
       <c r="N59" s="1"/>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14">
       <c r="A60" s="1" t="s">
         <v>44</v>
       </c>
@@ -5783,7 +5787,7 @@
       <c r="E60" s="1"/>
       <c r="N60" s="1"/>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:14">
       <c r="A61" s="1" t="s">
         <v>12</v>
       </c>
@@ -5794,7 +5798,7 @@
       <c r="E61" s="1"/>
       <c r="N61" s="1"/>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14">
       <c r="A62" s="1" t="s">
         <v>30</v>
       </c>
@@ -5805,7 +5809,7 @@
       <c r="E62" s="1"/>
       <c r="N62" s="1"/>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14">
       <c r="A63" s="1" t="s">
         <v>22</v>
       </c>
@@ -5816,7 +5820,7 @@
       <c r="E63" s="1"/>
       <c r="N63" s="1"/>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:14">
       <c r="A64" s="1" t="s">
         <v>20</v>
       </c>
@@ -5827,7 +5831,7 @@
       <c r="E64" s="1"/>
       <c r="N64" s="1"/>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:14">
       <c r="A65" s="1" t="s">
         <v>24</v>
       </c>
@@ -5838,7 +5842,7 @@
       <c r="E65" s="1"/>
       <c r="N65" s="1"/>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:14">
       <c r="A66" s="1" t="s">
         <v>14</v>
       </c>
@@ -5849,7 +5853,7 @@
       <c r="E66" s="1"/>
       <c r="N66" s="1"/>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:14">
       <c r="A67" s="1" t="s">
         <v>15</v>
       </c>
@@ -5860,7 +5864,7 @@
       <c r="E67" s="1"/>
       <c r="N67" s="1"/>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:14">
       <c r="A68" s="2" t="s">
         <v>36</v>
       </c>
@@ -5871,7 +5875,7 @@
       <c r="E68" s="1"/>
       <c r="N68" s="1"/>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:14">
       <c r="A69" s="1" t="s">
         <v>31</v>
       </c>
@@ -5882,7 +5886,7 @@
       <c r="E69" s="1"/>
       <c r="N69" s="1"/>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:14">
       <c r="A70" s="1" t="s">
         <v>33</v>
       </c>
@@ -5893,7 +5897,7 @@
       <c r="E70" s="1"/>
       <c r="N70" s="1"/>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:14">
       <c r="A71" s="1" t="s">
         <v>38</v>
       </c>
@@ -5904,29 +5908,164 @@
       <c r="E71" s="1"/>
       <c r="N71" s="1"/>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:14">
       <c r="A72" s="1"/>
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
       <c r="N72" s="1"/>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:14">
       <c r="A73" s="1"/>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
       <c r="N73" s="1"/>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:14">
       <c r="A74" s="1"/>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
       <c r="N74" s="1"/>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:14">
       <c r="C77" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="159">
+    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="L37:L38"/>
+    <mergeCell ref="L47:L48"/>
+    <mergeCell ref="L43:L46"/>
+    <mergeCell ref="L26:L27"/>
+    <mergeCell ref="L39:L40"/>
+    <mergeCell ref="D28:D30"/>
+    <mergeCell ref="D31:D33"/>
+    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="E28:E30"/>
+    <mergeCell ref="B9:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="B18:B33"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="N23:N25"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="M2:M4"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="N18:N19"/>
+    <mergeCell ref="N51:N52"/>
+    <mergeCell ref="L2:L4"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="L9:L11"/>
+    <mergeCell ref="L12:L13"/>
+    <mergeCell ref="L16:L17"/>
+    <mergeCell ref="L18:L19"/>
+    <mergeCell ref="L20:L22"/>
+    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="L51:L52"/>
+    <mergeCell ref="L23:L25"/>
+    <mergeCell ref="L28:L30"/>
+    <mergeCell ref="L31:L33"/>
+    <mergeCell ref="L34:L36"/>
+    <mergeCell ref="N34:N36"/>
+    <mergeCell ref="M12:M13"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="N31:N33"/>
+    <mergeCell ref="M28:M30"/>
+    <mergeCell ref="M41:M42"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="N9:N11"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="M51:M52"/>
+    <mergeCell ref="M47:M48"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="M20:M22"/>
+    <mergeCell ref="M23:M25"/>
+    <mergeCell ref="N12:N13"/>
+    <mergeCell ref="N20:N22"/>
+    <mergeCell ref="M14:M15"/>
+    <mergeCell ref="N14:N15"/>
+    <mergeCell ref="M26:M27"/>
+    <mergeCell ref="N26:N27"/>
+    <mergeCell ref="M39:M40"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="D23:D25"/>
+    <mergeCell ref="C34:C36"/>
+    <mergeCell ref="E34:E36"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="G23:G25"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="G31:G33"/>
+    <mergeCell ref="A9:A52"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="G51:G52"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="C43:C46"/>
+    <mergeCell ref="G47:G48"/>
+    <mergeCell ref="G49:G50"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="G37:G38"/>
+    <mergeCell ref="E23:E25"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="E31:E33"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="G20:G22"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="G41:G42"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="E49:E50"/>
+    <mergeCell ref="L49:L50"/>
+    <mergeCell ref="M49:M50"/>
+    <mergeCell ref="N49:N50"/>
+    <mergeCell ref="B47:B50"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="G39:G40"/>
+    <mergeCell ref="E43:E46"/>
+    <mergeCell ref="G43:G46"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="B43:B46"/>
+    <mergeCell ref="E47:E48"/>
+    <mergeCell ref="N47:N48"/>
+    <mergeCell ref="L41:L42"/>
+    <mergeCell ref="D43:D46"/>
+    <mergeCell ref="M43:M46"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="N43:N46"/>
     <mergeCell ref="N37:N38"/>
     <mergeCell ref="N41:N42"/>
     <mergeCell ref="N28:N30"/>
@@ -5951,141 +6090,6 @@
     <mergeCell ref="E20:E22"/>
     <mergeCell ref="E9:E11"/>
     <mergeCell ref="E12:E13"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="E49:E50"/>
-    <mergeCell ref="L49:L50"/>
-    <mergeCell ref="M49:M50"/>
-    <mergeCell ref="N49:N50"/>
-    <mergeCell ref="B47:B50"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="G39:G40"/>
-    <mergeCell ref="E43:E46"/>
-    <mergeCell ref="G43:G46"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="B43:B46"/>
-    <mergeCell ref="E47:E48"/>
-    <mergeCell ref="N47:N48"/>
-    <mergeCell ref="L41:L42"/>
-    <mergeCell ref="D43:D46"/>
-    <mergeCell ref="M43:M46"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="N43:N46"/>
-    <mergeCell ref="A2:A8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="G31:G33"/>
-    <mergeCell ref="A9:A52"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="G51:G52"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="C43:C46"/>
-    <mergeCell ref="G47:G48"/>
-    <mergeCell ref="G49:G50"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="G37:G38"/>
-    <mergeCell ref="E23:E25"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="E31:E33"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="G20:G22"/>
-    <mergeCell ref="E41:E42"/>
-    <mergeCell ref="G41:G42"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="M51:M52"/>
-    <mergeCell ref="M47:M48"/>
-    <mergeCell ref="C28:C30"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="M20:M22"/>
-    <mergeCell ref="M23:M25"/>
-    <mergeCell ref="N12:N13"/>
-    <mergeCell ref="N20:N22"/>
-    <mergeCell ref="M14:M15"/>
-    <mergeCell ref="N14:N15"/>
-    <mergeCell ref="M26:M27"/>
-    <mergeCell ref="N26:N27"/>
-    <mergeCell ref="M39:M40"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="D20:D22"/>
-    <mergeCell ref="D23:D25"/>
-    <mergeCell ref="C34:C36"/>
-    <mergeCell ref="E34:E36"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="G23:G25"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="N51:N52"/>
-    <mergeCell ref="L2:L4"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="L9:L11"/>
-    <mergeCell ref="L12:L13"/>
-    <mergeCell ref="L16:L17"/>
-    <mergeCell ref="L18:L19"/>
-    <mergeCell ref="L20:L22"/>
-    <mergeCell ref="L14:L15"/>
-    <mergeCell ref="L51:L52"/>
-    <mergeCell ref="L23:L25"/>
-    <mergeCell ref="L28:L30"/>
-    <mergeCell ref="L31:L33"/>
-    <mergeCell ref="L34:L36"/>
-    <mergeCell ref="N34:N36"/>
-    <mergeCell ref="M12:M13"/>
-    <mergeCell ref="N16:N17"/>
-    <mergeCell ref="N31:N33"/>
-    <mergeCell ref="M28:M30"/>
-    <mergeCell ref="M41:M42"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="N9:N11"/>
-    <mergeCell ref="M16:M17"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="B2:B6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="N23:N25"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="M2:M4"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="N18:N19"/>
-    <mergeCell ref="B34:B36"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="L37:L38"/>
-    <mergeCell ref="L47:L48"/>
-    <mergeCell ref="L43:L46"/>
-    <mergeCell ref="L26:L27"/>
-    <mergeCell ref="L39:L40"/>
-    <mergeCell ref="D28:D30"/>
-    <mergeCell ref="D31:D33"/>
-    <mergeCell ref="D34:D36"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="E28:E30"/>
-    <mergeCell ref="B9:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="B18:B33"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="D18:D19"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="F1:G1 F53:G54 F57:G1048576 F55:F56">

</xml_diff>